<commit_message>
add screenshot for readme.md
</commit_message>
<xml_diff>
--- a/KeywordPlannerAppData.xlsx
+++ b/KeywordPlannerAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhafner/Documents/Development/Apps/keywordGenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5321BEA5-EFE6-2449-A3C2-D419F50FB8EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C020DD-3254-8A40-87E6-6E5F6B4BA862}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="980" windowWidth="28040" windowHeight="16660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="580" windowWidth="28040" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Data Sheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="72">
   <si>
     <t>Keyword status</t>
   </si>
@@ -57,18 +57,9 @@
     <t>palm springs luxury hotels</t>
   </si>
   <si>
-    <t>palm springs hotels</t>
-  </si>
-  <si>
-    <t>ritz carlton rancho mirage</t>
-  </si>
-  <si>
     <t>REgular Hotel Keywords</t>
   </si>
   <si>
-    <t>vacation palm springs</t>
-  </si>
-  <si>
     <t>5 star hotels in palm springs</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>best places to stay in palm springs</t>
   </si>
   <si>
-    <t>ritz rancho mirage</t>
-  </si>
-  <si>
     <t>ritz carlton palm springs</t>
   </si>
   <si>
@@ -108,15 +96,9 @@
     <t>spa hotel palm springs</t>
   </si>
   <si>
-    <t>rancho mirage hotels</t>
-  </si>
-  <si>
     <t>palm springs resorts</t>
   </si>
   <si>
-    <t>ritz palm springs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Luxury </t>
   </si>
   <si>
@@ -211,6 +193,63 @@
   </si>
   <si>
     <t>Sum of Estimated Clicks</t>
+  </si>
+  <si>
+    <t>ergonomic</t>
+  </si>
+  <si>
+    <t>rolling</t>
+  </si>
+  <si>
+    <t>colorful</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>leather</t>
+  </si>
+  <si>
+    <t>plastic</t>
+  </si>
+  <si>
+    <t>modern</t>
+  </si>
+  <si>
+    <t>computer</t>
+  </si>
+  <si>
+    <t>wheeled</t>
+  </si>
+  <si>
+    <t>chair</t>
+  </si>
+  <si>
+    <t>desk chair</t>
+  </si>
+  <si>
+    <t>office chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seating </t>
+  </si>
+  <si>
+    <t>for sale</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>cheap</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>coupons</t>
+  </si>
+  <si>
+    <t>deals</t>
   </si>
 </sst>
 </file>
@@ -220,7 +259,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -355,6 +394,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -549,7 +594,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -689,19 +734,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </left>
@@ -780,19 +812,18 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -810,6 +841,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1703,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1725,7 +1757,7 @@
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1737,811 +1769,809 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>57</v>
+        <v>31</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>11</v>
+      <c r="C2" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="9" t="str">
-        <f>C2</f>
-        <v>5 star hotels in palm springs</v>
+        <f t="shared" ref="E2:E10" si="0">"''"&amp;C2&amp;"''"</f>
+        <v>''ergonomic''</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G2" s="7">
         <f ca="1">RANDBETWEEN(250,5000)</f>
-        <v>2605</v>
-      </c>
-      <c r="H2" s="21">
+        <v>2915</v>
+      </c>
+      <c r="H2" s="20">
         <f ca="1">RAND()/10</f>
-        <v>8.0146953835925683E-2</v>
-      </c>
-      <c r="I2" s="20">
+        <v>1.7396020652456233E-2</v>
+      </c>
+      <c r="I2" s="19">
         <f ca="1">+G2*H2</f>
-        <v>208.7828147425864</v>
+        <v>50.709400201909922</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>14</v>
+      <c r="C3" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="9" t="str">
-        <f t="shared" ref="E3:E13" si="0">C3</f>
-        <v>best hotels in palm springs</v>
+        <f t="shared" si="0"/>
+        <v>''rolling''</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" ref="G3:G25" ca="1" si="1">RANDBETWEEN(250,5000)</f>
-        <v>3257</v>
-      </c>
-      <c r="H3" s="21">
+        <v>3400</v>
+      </c>
+      <c r="H3" s="20">
         <f t="shared" ref="H3:H25" ca="1" si="2">RAND()/10</f>
-        <v>4.9337801048495181E-2</v>
-      </c>
-      <c r="I3" s="20">
+        <v>6.5658128304785443E-2</v>
+      </c>
+      <c r="I3" s="19">
         <f t="shared" ref="I3:I25" ca="1" si="3">+G3*H3</f>
-        <v>160.6932180149488</v>
+        <v>223.2376362362705</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>19</v>
+      <c r="C4" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>best places to stay in palm springs</v>
+        <v>''colorful''</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>2726</v>
-      </c>
-      <c r="H4" s="21">
+        <v>3422</v>
+      </c>
+      <c r="H4" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>9.6453798142448251E-3</v>
-      </c>
-      <c r="I4" s="20">
+        <v>3.4369344864595953E-2</v>
+      </c>
+      <c r="I4" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>26.293305373631394</v>
+        <v>117.61189812664735</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>17</v>
+      <c r="C5" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>best resorts in palm springs</v>
+        <v>''white''</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>4409</v>
-      </c>
-      <c r="H5" s="21">
+        <v>4917</v>
+      </c>
+      <c r="H5" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>6.3108200711551793E-2</v>
-      </c>
-      <c r="I5" s="20">
+        <v>4.9507745726353712E-2</v>
+      </c>
+      <c r="I5" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>278.24405693723185</v>
+        <v>243.42958573648122</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>16</v>
+      <c r="C6" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>best spas in palm springs</v>
+        <v>''leather''</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>1369</v>
-      </c>
-      <c r="H6" s="21">
+        <v>804</v>
+      </c>
+      <c r="H6" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>7.0137351479096013E-2</v>
-      </c>
-      <c r="I6" s="20">
+        <v>3.4678042294064057E-2</v>
+      </c>
+      <c r="I6" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>96.018034174882445</v>
+        <v>27.881146004427503</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>6</v>
+      <c r="C7" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>palm springs luxury hotels</v>
+        <v>''plastic''</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>2301</v>
-      </c>
-      <c r="H7" s="21">
+        <v>3234</v>
+      </c>
+      <c r="H7" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>4.511907436323093E-3</v>
-      </c>
-      <c r="I7" s="20">
+        <v>6.3546849727934202E-2</v>
+      </c>
+      <c r="I7" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>10.381899010979437</v>
+        <v>205.5105120201392</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>25</v>
+      <c r="C8" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>palm springs resorts</v>
+        <v>''modern''</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>4698</v>
-      </c>
-      <c r="H8" s="21">
+        <v>1576</v>
+      </c>
+      <c r="H8" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>6.8698162899651249E-2</v>
-      </c>
-      <c r="I8" s="20">
+        <v>2.1762001581872071E-2</v>
+      </c>
+      <c r="I8" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>322.7439693025616</v>
+        <v>34.296914493030386</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>4</v>
+      <c r="C9" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>palm springs spa</v>
+        <v>''computer''</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>2226</v>
-      </c>
-      <c r="H9" s="21">
+        <v>4132</v>
+      </c>
+      <c r="H9" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>3.9806856239473387E-2</v>
-      </c>
-      <c r="I9" s="20">
+        <v>9.6315326036134061E-2</v>
+      </c>
+      <c r="I9" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>88.610061989067759</v>
+        <v>397.97492718130593</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>13</v>
+      <c r="C10" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>palm springs spa resort</v>
+        <v>''wheeled''</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>845</v>
-      </c>
-      <c r="H10" s="21">
+        <v>4697</v>
+      </c>
+      <c r="H10" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>8.966984862817215E-2</v>
-      </c>
-      <c r="I10" s="20">
+        <v>6.7373611595124935E-2</v>
+      </c>
+      <c r="I10" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>75.771022090805459</v>
+        <v>316.45385366230181</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>spa hotel palm springs</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>1850</v>
-      </c>
-      <c r="H11" s="21">
+        <v>1558</v>
+      </c>
+      <c r="H11" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>6.934340927786474E-2</v>
-      </c>
-      <c r="I11" s="20">
+        <v>9.5973620717919775E-2</v>
+      </c>
+      <c r="I11" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>128.28530716404975</v>
+        <v>149.52690107851902</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>top hotels in palm springs</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>38</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>4833</v>
-      </c>
-      <c r="H12" s="21">
+        <v>2946</v>
+      </c>
+      <c r="H12" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3386697650684217E-2</v>
-      </c>
-      <c r="I12" s="20">
+        <v>2.615936270509055E-2</v>
+      </c>
+      <c r="I12" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>209.68790974575683</v>
+        <v>77.065482529196757</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>hotels in palm springs ca</v>
+        <f t="shared" ref="E13:E22" si="4">"''"&amp;C13&amp;"''"</f>
+        <v>''desk chair''</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G13" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>1635</v>
-      </c>
-      <c r="H13" s="21">
+        <v>4462</v>
+      </c>
+      <c r="H13" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>7.2394059396178809E-2</v>
-      </c>
-      <c r="I13" s="20">
+        <v>3.6599800842654816E-2</v>
+      </c>
+      <c r="I13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>118.36428711275235</v>
+        <v>163.3083113599258</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E14" s="9" t="str">
-        <f t="shared" ref="E14:E17" si="4">"''"&amp;C14&amp;"''"</f>
-        <v>''palm desert hotels''</v>
+        <f t="shared" si="4"/>
+        <v>''office chair''</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G14" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>4278</v>
-      </c>
-      <c r="H14" s="21">
+        <v>2352</v>
+      </c>
+      <c r="H14" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5352288603781728E-2</v>
-      </c>
-      <c r="I14" s="20">
+        <v>5.67757281267081E-2</v>
+      </c>
+      <c r="I14" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>65.677090646978229</v>
+        <v>133.53651255401746</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>7</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="E15" s="9" t="str">
         <f t="shared" si="4"/>
-        <v>''palm springs hotels''</v>
+        <v>''seating ''</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>3130</v>
-      </c>
-      <c r="H15" s="21">
+        <v>3835</v>
+      </c>
+      <c r="H15" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>6.3469153646826731E-2</v>
-      </c>
-      <c r="I15" s="20">
+        <v>7.3592329339000354E-2</v>
+      </c>
+      <c r="I15" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>198.65845091456768</v>
+        <v>282.22658301506635</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v>''rancho mirage hotels''</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>527</v>
-      </c>
-      <c r="H16" s="21">
+        <v>2725</v>
+      </c>
+      <c r="H16" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>4.1179771295491253E-2</v>
-      </c>
-      <c r="I16" s="20">
+        <v>6.2789588130876097E-3</v>
+      </c>
+      <c r="I16" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>21.70173947272389</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>17.110162765663738</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E17" s="9" t="str">
         <f t="shared" si="4"/>
-        <v>''vacation palm springs''</v>
+        <v>''for sale''</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>3942</v>
-      </c>
-      <c r="H17" s="21">
+        <v>4435</v>
+      </c>
+      <c r="H17" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>4.882224243286596E-2</v>
-      </c>
-      <c r="I17" s="20">
+        <v>1.7714579506428917E-2</v>
+      </c>
+      <c r="I17" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>192.45727967035762</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>78.564160111012242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E18" s="9" t="str">
-        <f>"+"&amp;SUBSTITUTE(C18," "," +")</f>
-        <v>+ritz +carlton +palm +springs</v>
+        <f t="shared" si="4"/>
+        <v>''discount''</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G18" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>2271</v>
-      </c>
-      <c r="H18" s="21">
+        <v>479</v>
+      </c>
+      <c r="H18" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2042368622905275E-2</v>
-      </c>
-      <c r="I18" s="20">
+        <v>1.2773338380882215E-2</v>
+      </c>
+      <c r="I18" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>27.348219142617882</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6.1184290844425808</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E19" s="9" t="str">
-        <f t="shared" ref="E19:E21" si="5">"+"&amp;SUBSTITUTE(C19," "," +")</f>
-        <v>+ritz +carlton +rancho +mirage</v>
+        <f t="shared" si="4"/>
+        <v>''cheap''</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>1325</v>
-      </c>
-      <c r="H19" s="21">
+        <v>4065</v>
+      </c>
+      <c r="H19" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4967323454859714E-2</v>
-      </c>
-      <c r="I19" s="20">
+        <v>6.0326680077647875E-2</v>
+      </c>
+      <c r="I19" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>46.331703577689119</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>245.2279545156386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E20" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>+ritz +palm +springs</v>
+        <f t="shared" si="4"/>
+        <v>''online''</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G20" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>2338</v>
-      </c>
-      <c r="H20" s="21">
+        <v>1852</v>
+      </c>
+      <c r="H20" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>1.7507583443144736E-2</v>
-      </c>
-      <c r="I20" s="20">
+        <v>2.2099378746560306E-2</v>
+      </c>
+      <c r="I20" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>40.932730090072397</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>40.928049438629685</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E21" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>+ritz +rancho +mirage</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>33</v>
+        <f t="shared" si="4"/>
+        <v>''coupons''</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="G21" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>2574</v>
-      </c>
-      <c r="H21" s="21">
+        <v>1338</v>
+      </c>
+      <c r="H21" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>7.5407738399849419E-2</v>
-      </c>
-      <c r="I21" s="20">
+        <v>9.7036021677404702E-2</v>
+      </c>
+      <c r="I21" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>194.0995186412124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>129.8341970043675</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E22" s="9" t="str">
-        <f>+"["&amp;C22&amp;"]"</f>
-        <v>[ritz carlton palm springs]</v>
+        <f t="shared" si="4"/>
+        <v>''deals''</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G22" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>1887</v>
-      </c>
-      <c r="H22" s="21">
+        <v>2172</v>
+      </c>
+      <c r="H22" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>8.8001311048613556E-2</v>
-      </c>
-      <c r="I22" s="20">
+        <v>4.8613632801689052E-2</v>
+      </c>
+      <c r="I22" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>166.05847394873379</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>105.58881044526862</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="C23" s="9"/>
       <c r="D23" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E23" s="9" t="str">
-        <f t="shared" ref="E23:E25" si="6">+"["&amp;C23&amp;"]"</f>
-        <v>[ritz carlton rancho mirage]</v>
+        <f t="shared" ref="E23:E25" si="5">+"["&amp;C23&amp;"]"</f>
+        <v>[]</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>3715</v>
-      </c>
-      <c r="H23" s="21">
+        <v>716</v>
+      </c>
+      <c r="H23" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>5.9566395681747111E-2</v>
-      </c>
-      <c r="I23" s="20">
+        <v>1.998805485238412E-2</v>
+      </c>
+      <c r="I23" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>221.28915995769052</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>14.31144727430703</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="C24" s="9"/>
       <c r="D24" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E24" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>[ritz palm springs]</v>
+        <f t="shared" si="5"/>
+        <v>[]</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>3388</v>
-      </c>
-      <c r="H24" s="21">
+        <v>4978</v>
+      </c>
+      <c r="H24" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0913842561797726E-2</v>
-      </c>
-      <c r="I24" s="20">
+        <v>2.2751069387345668E-2</v>
+      </c>
+      <c r="I24" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>36.976098599370694</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>113.25482341020674</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="C25" s="12"/>
       <c r="D25" s="12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E25" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>[ritz rancho mirage]</v>
+        <f t="shared" si="5"/>
+        <v>[]</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G25" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>3434</v>
-      </c>
-      <c r="H25" s="21">
+        <v>2066</v>
+      </c>
+      <c r="H25" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>1.0235559696318886E-2</v>
-      </c>
-      <c r="I25" s="20">
+        <v>2.455438922741009E-2</v>
+      </c>
+      <c r="I25" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>35.148911997159054</v>
+        <v>50.729368143829248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C27" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2565,282 +2595,282 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="21">
+        <v>3071.5907967612757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="21">
+        <v>1600.6388130251541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="21">
+        <v>1600.6388130251541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="21">
+        <v>262.87831223135413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="21">
+        <v>114.39451630138574</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="21">
+        <v>3.1045697722176886</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="21">
+        <v>104.36844111210574</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="21">
+        <v>134.86463784909691</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="21">
+        <v>154.5410689811585</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="21">
+        <v>192.92988502071589</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="21">
+        <v>283.85107859139634</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="21">
+        <v>52.979869331161304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="21">
+        <v>108.10114597865525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="21">
+        <v>188.62528785590669</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="21">
+        <v>541.75852248235753</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="21">
+        <v>104.287350752728</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="21">
+        <v>104.287350752728</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="21">
+        <v>437.47117172962953</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="21">
+        <v>259.35814813505499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="21">
+        <v>20.782024696511613</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="21">
+        <v>105.87489365839517</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="21">
+        <v>51.456105239667764</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="21">
+        <v>929.19346125376399</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="21">
+        <v>766.49259521139595</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="21">
+        <v>47.486122978372933</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="21">
+        <v>363.13784890712503</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="21">
+        <v>280.3989713871311</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="21">
+        <v>75.469651938766887</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="21">
+        <v>162.70086604236809</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="22">
-        <v>3071.5907967612757</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="22">
-        <v>1600.6388130251541</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="22">
-        <v>1600.6388130251541</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="22">
-        <v>262.87831223135413</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="22">
-        <v>114.39451630138574</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="22">
-        <v>3.1045697722176886</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="22">
-        <v>104.36844111210574</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="22">
-        <v>134.86463784909691</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="22">
-        <v>154.5410689811585</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="22">
-        <v>192.92988502071589</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="22">
-        <v>283.85107859139634</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="22">
-        <v>52.979869331161304</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="22">
-        <v>108.10114597865525</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="22">
-        <v>188.62528785590669</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="22">
-        <v>541.75852248235753</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="22">
-        <v>104.287350752728</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="22">
-        <v>104.287350752728</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="22">
-        <v>437.47117172962953</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
+      <c r="B33" s="21">
+        <v>26.841184198988664</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="21">
+        <v>46.281555245998575</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="22">
-        <v>259.35814813505499</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+      <c r="B35" s="21">
+        <v>47.150199365818985</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="22">
-        <v>20.782024696511613</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="22">
-        <v>105.87489365839517</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="22">
-        <v>51.456105239667764</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="22">
-        <v>929.19346125376399</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="22">
-        <v>766.49259521139595</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="22">
-        <v>47.486122978372933</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="22">
-        <v>363.13784890712503</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="22">
-        <v>280.3989713871311</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="22">
-        <v>75.469651938766887</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
+      <c r="B36" s="21">
+        <v>42.42792723156186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="22">
-        <v>162.70086604236809</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="22">
-        <v>26.841184198988664</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="22">
-        <v>46.281555245998575</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="22">
-        <v>47.150199365818985</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="22">
-        <v>42.42792723156186</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="22">
+      <c r="B37" s="21">
         <v>3071.5907967612757</v>
       </c>
     </row>
@@ -2864,28 +2894,28 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2897,7 +2927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2919,10 +2949,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2930,17 +2960,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D3" s="5" t="str">
         <f>+"["&amp;B3&amp;"]"</f>
         <v>[ritz carlton palm springs]</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2948,17 +2978,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="str">
         <f t="shared" ref="D4" si="0">"''"&amp;B4&amp;"''"</f>
         <v>''palm desert hotels''</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2966,17 +2996,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="5" t="str">
         <f>"+"&amp;SUBSTITUTE(B5," "," +")</f>
         <v>+ritz +carlton +palm +springs</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2984,7 +3014,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>5</v>
@@ -2994,7 +3024,7 @@
         <v>5 star hotels in palm springs</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>